<commit_message>
Major update : FHCG created
</commit_message>
<xml_diff>
--- a/YEFIKIR_MAID_TERA/UNDER_DEVELOPMENT/የየእሑድ_ዝክር_የበዓላት_ዝርዝር_የዓመት_____Modified_Result.xlsx
+++ b/YEFIKIR_MAID_TERA/UNDER_DEVELOPMENT/የየእሑድ_ዝክር_የበዓላት_ዝርዝር_የዓመት_____Modified_Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ab/Desktop/JA-COLAB/JA-COLAB/YEFIKIR_MAID_TERA/UNDER_DEVELOPMENT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70F19CC-A319-C54B-B2C5-3B1ABAC5A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BED4E2-9F36-B043-8B0F-21F10311D5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="640" windowWidth="26720" windowHeight="18900" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3520" yWindow="640" windowWidth="26720" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="የየእሑድ ዝክር የበዓላት ዝርዝር (2)" sheetId="1" r:id="rId1"/>
@@ -130,18 +130,6 @@
 ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ሐምሌ  2</t>
   </si>
   <si>
-    <t>ዘካሪ፥ ወንድ እና ሴት
-የሚዘከረው በዓል እና ቀኑ፥  7   አጋዕዝተ አለም ስላሴ ፣ዲዎስቆሮስ  
-ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 13
-ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  7</t>
-  </si>
-  <si>
-    <t>ዘካሪ: ነብያት ግደይና ሀይማኖት ፀሀይ
- የሚዘከረው በዓል እና ቀኑ:  3   ቅዱስ ሩፋኤል 
- ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  September 10
- ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ: ጳጉሜ ፭</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8: '  |4   ዮሐንስ ወልደ ነጎድጓድ ፣አባ መቃርዎስ፣ አባ አብርሐ  |5   ጴጥሮስና ጳውሎስ ፣ገብረ መንፈስ ቅዱስ  |6   ቁስቋም ፣ኢየሱስ ፣አርሴማ ቅድስት ፣እያሱ  |7   አጋዕዝተ አለም ስላሴ ፣ዲዎስቆሮስ  |8   ኪሮስ ፣ማቲዮስ፣ ኪሩቤል አርባእቱ እንስሳ፡ ዘካርያስ  |9   ሰልስቱ ምዕት፣ ቶማስ ፣እስትንፋሰ ክርስቶስ ፣አትናትዮስ  |10   መስቀለ ክርስቶስ ፣ናትናኤል ሐዋርያ ፣ፀደንያ ማርያም'</t>
   </si>
   <si>
@@ -191,12 +179,6 @@
 የሚዘከረው በዓል እና ቀኑ፥  9   ሰልስቱ ምዕት፣ ቶማስ ፣እስትንፋሰ ክርስቶስ ፣አትናትዮስ  
 ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  July 16
 ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ሐምሌ  9</t>
-  </si>
-  <si>
-    <t>ዘካሪ፥ ወንድ እና ሴት
-የሚዘከረው በዓል እና ቀኑ፥  14   አቡነ አረጋዊ ፣ገብረ ክርስቶስ/ገብረ መርአዊ/ ዘሚካኤል ፣ሙሴ ፀሊም  
-ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 20
-ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  14</t>
   </si>
   <si>
     <t xml:space="preserve"> 15: '  |11   ሐና እና ኢያቄም ፣አቡነ ሐራ  |12   ሚካኤል፣ አባ ሳሙኤልና ፣ ናትናኤል ሐዋርያ  |13   ፀጋ ኢየሱስ/ ዘርአ ብሩክ/ ፣ሩፋኤል ፣እግዚአብሔር አብ  |14   አቡነ አረጋዊ ፣ገብረ ክርስቶስ/ገብረ መርአዊ/ ዘሚካኤል ፣ሙሴ ፀሊም  |15   ቂርቆስና እየሉጣ ፣ሚናስ  |16   ኪዳነ ምህረት ፣ኤልሳቤጥ  |17   እስጢፋኖስ ፣ገሪማ ፣ወለተ ጴጥሮስ ፣አቡነ በትረ ማርያም ፣ ያዕቆብ ወልደ ዘብዲዮስ ፣ሙሴ'</t>
@@ -252,12 +234,6 @@
 ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ሐምሌ  16</t>
   </si>
   <si>
-    <t>ዘካሪ፥ ወንድ እና ሴት
-የሚዘከረው በዓል እና ቀኑ፥  21   ቅድስት ድንግል ማርያም  
-ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 27
-ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  21</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 22: '  |18   ማዕቀብ አልፋ ፣ኢዩስጣቲዮስ ፣ፊሊጶስ  |19   ገብርኤል ፣ስልስቱ ደቂቅ፣ ይመርሐነ ክርስቶስ  |20   ዮሐንስ  ሀፂር ፤ሕንፀተ ቤተ ክርስቲያን  |21   ቅድስት ድንግል ማርያም  |22   ሉቃስ ፣ደቅስዮስ ፣ኡራኤል ፣ ብስራተ ገብርኤል  |23   ቅዱስ ማር ጊዮርጊስ  |24   ተክለ ሐይማኖት ፣ጎርጎርዮስ ፣24ቱ ካህናተ ሰማይ፣ ክርስረቶስ ሰምራ'</t>
   </si>
   <si>
@@ -313,12 +289,6 @@
 ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ሐምሌ  23</t>
   </si>
   <si>
-    <t>ዘካሪ፥ ወንድ እና ሴት
-የሚዘከረው በዓል እና ቀኑ፥  28   አማኑኤል ፣ አበው አብርሃም ይህሳቅ ያዕቆብ    
-ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  September 03
-ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  28</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 29: '  |25   ቅዱስ መርቆሬዎስ ፣አቡነ ሀቢብ  |26   ዮሴፍ፣ ቶማስ ዘህንደኬ፣ አቡነ ሀብተ ማርያም  |27   መድሐኔአለም ፣አቡነ መባዓ ፅዮን ተክለ አልፋማርያም  |28   አማኑኤል ፣ አበው አብርሃም ይህሳቅ ያዕቆብ    |29   በዓለ እግዚአብሔር (በዓለወልድ)፣ቅዱስ ላሊበላ ፣ቅድስት አርሴማ  |30   ቅዱስ ማርቆስ ፡ ዮሐንስ መጥምቅ  |1   ልደታ፣ዮሐንስ ፣ራጉኤል ፣እዮብ ፣ኤልያስ ፣ ሶስና'}</t>
   </si>
   <si>
@@ -1664,12 +1634,139 @@
   <si>
     <t> 11.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ዘካሪ፥ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ደጁ እና ማስረሻ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+የሚዘከረው በዓል እና ቀኑ፥  7   አጋዕዝተ አለም ስላሴ ፣ዲዎስቆሮስ  
+ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 13
+ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ዘካሪ፥ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>በፍቃዱ እና ቤተልሔም አበበ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+የሚዘከረው በዓል እና ቀኑ፥  14   አቡነ አረጋዊ ፣ገብረ ክርስቶስ/ገብረ መርአዊ/ ዘሚካኤል ፣ሙሴ ፀሊም  
+ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 20
+ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ዘካሪ፥ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ቤዛዊት አሰፋ፣ እፀገነት አሰፋ እና እዮብ አሰፋ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+የሚዘከረው በዓል እና ቀኑ፥  21   ቅድስት ድንግል ማርያም  
+ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  August 27
+ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ዘካሪ፥ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ኢሳይያስ እና ቤተልሔም ሙሉ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+የሚዘከረው በዓል እና ቀኑ፥  28   አማኑኤል ፣ አበው አብርሃም ይህሳቅ ያዕቆብ    
+ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  September 03
+ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ፥ ነሐሴ  28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ዘካሪ: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>ነቢያት ግደይና ሀይማኖት ፀሀይ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ የሚዘከረው በዓል እና ቀኑ:  3   ቅዱስ ሩፋኤል 
+ ጸበል ጻዲቅ የሚቀርብበት ቀን በውጭ:  September 10
+ ጸበል ጻዲቅ የሚቀርብበት ቀን በኢትዮጵያ: ጳጉሜ ፭</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1765,6 +1862,12 @@
       <name val="Calibri (Body)"/>
     </font>
     <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
@@ -1796,6 +1899,12 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1946,11 +2055,11 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1962,10 +2071,10 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2313,7 +2422,7 @@
   </sheetPr>
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="81" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -2410,144 +2519,144 @@
         <v>23</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>24</v>
+        <v>479</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>25</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="158" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="F3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="G3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="H3" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="K3" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="54" t="s">
-        <v>35</v>
-      </c>
       <c r="L3" s="55" t="s">
-        <v>36</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="165" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="E4" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="F4" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="G4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="H4" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="I4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="K4" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="54" t="s">
-        <v>46</v>
-      </c>
       <c r="L4" s="55" t="s">
-        <v>47</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="211" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="G5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="H5" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="I5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="K5" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="54" t="s">
-        <v>57</v>
-      </c>
       <c r="L5" s="55" t="s">
-        <v>58</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="175" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="54" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -2560,7 +2669,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="H11" s="42" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="13:25" ht="24" customHeight="1">
@@ -2655,7 +2764,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" fitToWidth="3" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="72" fitToWidth="3" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2663,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2676,365 +2785,366 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" customHeight="1">
       <c r="A2" s="49" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" customHeight="1">
       <c r="A3" s="49" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" customHeight="1">
       <c r="A4" s="49" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1">
       <c r="A6" s="49" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" customHeight="1">
       <c r="A7" s="49" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" customHeight="1">
       <c r="A8" s="49" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" customHeight="1">
       <c r="A9" s="49" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" customHeight="1">
       <c r="A10" s="49" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1">
       <c r="A12" s="49" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" customHeight="1">
       <c r="A13" s="49" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1">
       <c r="A14" s="49" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1">
       <c r="A15" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" customHeight="1">
       <c r="B16" s="49" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="17" customHeight="1">
       <c r="B17" s="49" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="17" customHeight="1">
       <c r="B18" s="49" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="17" customHeight="1">
       <c r="B19" s="49" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="17" customHeight="1">
       <c r="B20" s="49" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="17" customHeight="1">
       <c r="B21" s="49" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="17" customHeight="1">
       <c r="B22" s="49" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="17" customHeight="1">
       <c r="B23" s="49" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="17">
       <c r="D25" s="49" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="17">
       <c r="D26" s="49" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="17">
       <c r="D27" s="49" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="17">
       <c r="D28" s="49" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="17">
       <c r="D29" s="49" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="17">
       <c r="D30" s="49" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="17">
       <c r="D31" s="49" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="17">
       <c r="D32" s="49" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="17">
       <c r="D33" s="49" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17">
       <c r="D34" s="49" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="17">
       <c r="D35" s="49" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17">
       <c r="D36" s="49" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17">
       <c r="D37" s="49" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="4:4" ht="17">
       <c r="D38" s="49" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="40" spans="4:4" ht="17">
       <c r="D40" s="49" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="41" spans="4:4" ht="17">
       <c r="D41" s="49" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="4:4" ht="17">
       <c r="D42" s="49" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="43" spans="4:4" ht="17">
       <c r="D43" s="49" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="44" spans="4:4" ht="17">
       <c r="D44" s="49" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="45" spans="4:4" ht="17">
       <c r="D45" s="49" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="46" spans="4:4" ht="17">
       <c r="D46" s="49" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="4:4" ht="17">
       <c r="D47" s="49" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="48" spans="4:4" ht="17">
       <c r="D48" s="49" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="17">
       <c r="D49" s="49" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="50" spans="4:4" ht="17">
       <c r="D50" s="49" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="51" spans="4:4" ht="17">
       <c r="D51" s="49" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3051,11 +3161,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3063,7 +3174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScale="63" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="63" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3129,19 +3240,19 @@
         <v>14</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -3150,148 +3261,148 @@
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="175" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="200" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="175" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="175" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -3453,27 +3564,27 @@
     </row>
     <row r="2" spans="1:12" ht="126" customHeight="1">
       <c r="D2" s="38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="126" customHeight="1">
       <c r="D3" s="38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="126" customHeight="1">
       <c r="D4" s="38" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="126" customHeight="1">
       <c r="D5" s="38" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="126" customHeight="1">
       <c r="D6" s="38" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="3:12" s="38" customFormat="1" ht="25" customHeight="1">
@@ -3540,32 +3651,32 @@
     </row>
     <row r="2" spans="1:21" ht="325" customHeight="1">
       <c r="A2" s="32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="R2" s="38"/>
       <c r="S2" s="2"/>
       <c r="T2" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="154" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="R3" s="38"/>
       <c r="S3" s="38"/>
@@ -3574,35 +3685,35 @@
     </row>
     <row r="4" spans="1:21" ht="409.5" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="R4" s="50" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="S4" s="38"/>
       <c r="T4" s="32" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="U4" s="38"/>
     </row>
     <row r="5" spans="1:21" ht="288" customHeight="1">
       <c r="A5" s="32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="R5" s="51" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="S5" s="38"/>
       <c r="T5" s="38"/>
@@ -3611,11 +3722,11 @@
     <row r="6" spans="1:21" ht="183" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2"/>
       <c r="R6" s="52" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="S6" s="38"/>
       <c r="T6" s="38"/>
@@ -3623,7 +3734,7 @@
     </row>
     <row r="7" spans="1:21" ht="182" customHeight="1">
       <c r="R7" s="52" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="S7" s="38"/>
       <c r="T7" s="38"/>
@@ -3631,17 +3742,17 @@
     </row>
     <row r="8" spans="1:21" ht="234" customHeight="1">
       <c r="R8" s="52" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="S8" s="38" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
     </row>
     <row r="9" spans="1:21" ht="234" customHeight="1">
       <c r="R9" s="53" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="S9" s="38"/>
       <c r="T9" s="38"/>
@@ -3649,7 +3760,7 @@
     </row>
     <row r="10" spans="1:21" ht="208" customHeight="1">
       <c r="R10" s="52" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="S10" s="38"/>
       <c r="T10" s="38"/>
@@ -3657,7 +3768,7 @@
     </row>
     <row r="11" spans="1:21" ht="286" customHeight="1">
       <c r="R11" s="52" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S11" s="38"/>
       <c r="T11" s="38"/>
@@ -3665,7 +3776,7 @@
     </row>
     <row r="12" spans="1:21" ht="260" customHeight="1">
       <c r="R12" s="52" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -3673,7 +3784,7 @@
     </row>
     <row r="13" spans="1:21" ht="409.5" customHeight="1">
       <c r="R13" s="52" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -3681,7 +3792,7 @@
     </row>
     <row r="14" spans="1:21" ht="286" customHeight="1">
       <c r="R14" s="52" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="S14" s="38"/>
       <c r="T14" s="38"/>
@@ -3689,7 +3800,7 @@
     </row>
     <row r="15" spans="1:21" ht="260" customHeight="1">
       <c r="R15" s="52" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="S15" s="38"/>
       <c r="T15" s="38"/>
@@ -3697,7 +3808,7 @@
     </row>
     <row r="16" spans="1:21" ht="260" customHeight="1">
       <c r="R16" s="52" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
@@ -3705,7 +3816,7 @@
     </row>
     <row r="17" spans="18:21" ht="260" customHeight="1">
       <c r="R17" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="S17" s="38"/>
       <c r="T17" s="38"/>
@@ -3713,7 +3824,7 @@
     </row>
     <row r="18" spans="18:21" ht="182" customHeight="1">
       <c r="R18" s="52" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="S18" s="38"/>
       <c r="T18" s="38"/>
@@ -3721,7 +3832,7 @@
     </row>
     <row r="19" spans="18:21" ht="234" customHeight="1">
       <c r="R19" s="52" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="S19" s="38"/>
       <c r="T19" s="38"/>
@@ -3729,7 +3840,7 @@
     </row>
     <row r="20" spans="18:21" ht="260" customHeight="1">
       <c r="R20" s="52" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="S20" s="38"/>
       <c r="T20" s="38"/>
@@ -3737,7 +3848,7 @@
     </row>
     <row r="21" spans="18:21" ht="260" customHeight="1">
       <c r="R21" s="52" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
@@ -3745,7 +3856,7 @@
     </row>
     <row r="22" spans="18:21" ht="234" customHeight="1">
       <c r="R22" s="52" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
@@ -3753,7 +3864,7 @@
     </row>
     <row r="23" spans="18:21" ht="156" customHeight="1">
       <c r="R23" s="52" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="S23" s="38"/>
       <c r="T23" s="38"/>
@@ -3761,7 +3872,7 @@
     </row>
     <row r="24" spans="18:21" ht="338" customHeight="1">
       <c r="R24" s="53" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="S24" s="38"/>
       <c r="T24" s="38"/>
@@ -3769,7 +3880,7 @@
     </row>
     <row r="25" spans="18:21" ht="234" customHeight="1">
       <c r="R25" s="53" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="S25" s="38"/>
       <c r="T25" s="38"/>
@@ -3777,7 +3888,7 @@
     </row>
     <row r="26" spans="18:21" ht="338" customHeight="1">
       <c r="R26" s="52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
@@ -3785,7 +3896,7 @@
     </row>
     <row r="27" spans="18:21" ht="182" customHeight="1">
       <c r="R27" s="53" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="S27" s="38"/>
       <c r="T27" s="38"/>
@@ -3793,7 +3904,7 @@
     </row>
     <row r="28" spans="18:21" ht="182" customHeight="1">
       <c r="R28" s="52" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="S28" s="38"/>
       <c r="T28" s="38"/>
@@ -3801,7 +3912,7 @@
     </row>
     <row r="29" spans="18:21" ht="208" customHeight="1">
       <c r="R29" s="52" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="S29" s="38"/>
       <c r="T29" s="38"/>
@@ -3809,7 +3920,7 @@
     </row>
     <row r="30" spans="18:21" ht="409.5" customHeight="1">
       <c r="R30" s="52" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="S30" s="38"/>
       <c r="T30" s="38"/>
@@ -3817,7 +3928,7 @@
     </row>
     <row r="31" spans="18:21" ht="182" customHeight="1">
       <c r="R31" s="52" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="S31" s="38"/>
       <c r="T31" s="38"/>
@@ -3825,7 +3936,7 @@
     </row>
     <row r="32" spans="18:21" ht="182" customHeight="1">
       <c r="R32" s="52" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="S32" s="38"/>
       <c r="T32" s="38"/>
@@ -3833,7 +3944,7 @@
     </row>
     <row r="33" spans="18:21" ht="234" customHeight="1">
       <c r="R33" s="52" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
@@ -3841,7 +3952,7 @@
     </row>
     <row r="34" spans="18:21" ht="208" customHeight="1">
       <c r="R34" s="52" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="S34" s="38"/>
       <c r="T34" s="38"/>
@@ -3863,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:I70"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A4" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3879,25 +3990,25 @@
   <sheetData>
     <row r="2" spans="2:9" ht="18" customHeight="1">
       <c r="B2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -3906,16 +4017,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="22" customFormat="1" ht="18" customHeight="1">
@@ -3923,10 +4034,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -3938,10 +4049,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -3953,13 +4064,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -3970,10 +4081,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -3985,20 +4096,20 @@
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:9" s="14" customFormat="1" ht="18" customHeight="1">
@@ -4006,19 +4117,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H9" s="13"/>
     </row>
@@ -4027,10 +4138,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -4042,10 +4153,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -4057,13 +4168,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -4074,16 +4185,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="18" customHeight="1">
@@ -4091,19 +4202,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H14" s="6"/>
     </row>
@@ -4112,18 +4223,18 @@
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="18" customHeight="1">
@@ -4131,10 +4242,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4146,10 +4257,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -4161,18 +4272,18 @@
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="20" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1">
@@ -4180,16 +4291,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1">
@@ -4197,10 +4308,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -4212,10 +4323,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -4227,10 +4338,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -4242,10 +4353,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -4257,10 +4368,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -4272,10 +4383,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -4287,16 +4398,16 @@
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" customHeight="1">
@@ -4304,10 +4415,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -4319,10 +4430,10 @@
         <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -4334,10 +4445,10 @@
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -4349,10 +4460,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -4364,10 +4475,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -4379,16 +4490,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="18" customHeight="1">
@@ -4396,10 +4507,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -4411,13 +4522,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="5" t="s">
@@ -4430,10 +4541,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -4445,10 +4556,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -4460,13 +4571,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -4477,16 +4588,16 @@
         <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="2:8" s="22" customFormat="1" ht="18" customHeight="1">
@@ -4494,19 +4605,19 @@
         <v>37</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H39" s="21"/>
     </row>
@@ -4515,10 +4626,10 @@
         <v>38</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -4530,20 +4641,20 @@
         <v>39</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="18" customHeight="1">
@@ -4551,10 +4662,10 @@
         <v>40</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -4566,16 +4677,16 @@
         <v>41</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
@@ -4585,10 +4696,10 @@
         <v>42</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -4600,10 +4711,10 @@
         <v>43</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -4615,10 +4726,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -4630,10 +4741,10 @@
         <v>45</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -4645,10 +4756,10 @@
         <v>46</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -4660,19 +4771,19 @@
         <v>47</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H49" s="6"/>
     </row>
@@ -4681,10 +4792,10 @@
         <v>48</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -4696,10 +4807,10 @@
         <v>49</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -4711,10 +4822,10 @@
         <v>50</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
@@ -4726,10 +4837,10 @@
         <v>51</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -4741,10 +4852,10 @@
         <v>52</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -4756,10 +4867,10 @@
         <v>53</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -4771,10 +4882,10 @@
         <v>54</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -4786,10 +4897,10 @@
         <v>55</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -4801,10 +4912,10 @@
         <v>56</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -4816,10 +4927,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -4831,10 +4942,10 @@
         <v>58</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
@@ -4846,10 +4957,10 @@
         <v>59</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -4861,10 +4972,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -4876,10 +4987,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -4891,10 +5002,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -4906,10 +5017,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
@@ -4921,13 +5032,13 @@
         <v>64</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E66" s="47" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
@@ -4938,18 +5049,18 @@
         <v>65</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E67" s="47" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="2:8">
@@ -4957,7 +5068,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="2:8">
@@ -4965,15 +5076,15 @@
         <v>67</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1">
       <c r="C70" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E70" s="48" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -5000,344 +5111,344 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="18" customHeight="1">
       <c r="B33" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="18" customHeight="1">
       <c r="B34" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="18" customHeight="1">
       <c r="B35" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="18" customHeight="1">
       <c r="B36" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -5361,28 +5472,28 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>327</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -5396,21 +5507,21 @@
         <v>44627.654004629629</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
       <c r="F2" s="27" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
@@ -5424,20 +5535,20 @@
         <v>44662.63244212963</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D3" s="25">
         <v>2025700783</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
@@ -5452,23 +5563,23 @@
         <v>44662.68240740741</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D4" s="30">
         <v>2027499750</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
@@ -5482,25 +5593,25 @@
         <v>44678.683888888889</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D5" s="30">
         <v>2022767789</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
@@ -5514,20 +5625,20 @@
         <v>44678.704641203702</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D6" s="25">
         <v>2405477070</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -5542,20 +5653,20 @@
         <v>44682.815486111111</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D7" s="25">
         <v>2024683349</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -5570,20 +5681,20 @@
         <v>44696.766817129632</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D8" s="25">
         <v>2025944122</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -5599,17 +5710,17 @@
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D9" s="25">
         <v>2028767811</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -5625,17 +5736,17 @@
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D10" s="25">
         <v>2025602453</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -5651,17 +5762,17 @@
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="25" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D11" s="25">
         <v>3016408908</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -5677,17 +5788,17 @@
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="25" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D12" s="25">
         <v>5756508771</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -5703,20 +5814,20 @@
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D13" s="25">
         <v>2025097423</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>353</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>358</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="6"/>
@@ -5731,19 +5842,19 @@
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -7399,7 +7510,7 @@
     </row>
     <row r="2" spans="1:25" ht="45" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -7441,25 +7552,25 @@
     </row>
     <row r="4" spans="1:25" ht="19" customHeight="1">
       <c r="A4" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>368</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -7478,25 +7589,25 @@
     </row>
     <row r="5" spans="1:25" ht="19" customHeight="1">
       <c r="A5" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>370</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>375</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -7515,25 +7626,25 @@
     </row>
     <row r="6" spans="1:25" ht="19" customHeight="1">
       <c r="A6" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="G6" s="18" t="s">
         <v>377</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>380</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>382</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -7552,25 +7663,25 @@
     </row>
     <row r="7" spans="1:25" ht="19" customHeight="1">
       <c r="A7" s="16" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -7589,25 +7700,25 @@
     </row>
     <row r="8" spans="1:25" ht="19" customHeight="1">
       <c r="A8" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>385</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>388</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>389</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>390</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -7628,7 +7739,7 @@
       <c r="A9" s="16"/>
       <c r="B9" s="6"/>
       <c r="C9" s="17" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -7697,7 +7808,7 @@
     </row>
     <row r="12" spans="1:25" ht="45" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -7739,25 +7850,25 @@
     </row>
     <row r="14" spans="1:25" ht="19" customHeight="1">
       <c r="A14" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="G14" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>368</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -7776,25 +7887,25 @@
     </row>
     <row r="15" spans="1:25" ht="19" customHeight="1">
       <c r="A15" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>374</v>
-      </c>
       <c r="G15" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -7813,25 +7924,25 @@
     </row>
     <row r="16" spans="1:25" ht="45" customHeight="1">
       <c r="A16" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>377</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>380</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>382</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -7840,7 +7951,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
@@ -7856,25 +7967,25 @@
     </row>
     <row r="17" spans="1:25" ht="19" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -7897,25 +8008,25 @@
     </row>
     <row r="18" spans="1:25" ht="19" customHeight="1">
       <c r="A18" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>385</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>388</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>389</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>390</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -7924,25 +8035,25 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="O18" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="R18" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="S18" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="O18" s="36" t="s">
+      <c r="T18" s="16" t="s">
         <v>363</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q18" s="16" t="s">
-        <v>365</v>
-      </c>
-      <c r="R18" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="S18" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="T18" s="16" t="s">
-        <v>368</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -7965,25 +8076,25 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="O19" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q19" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="R19" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="S19" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="O19" s="36" t="s">
-        <v>393</v>
-      </c>
-      <c r="P19" s="16" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="R19" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>374</v>
-      </c>
       <c r="T19" s="16" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
@@ -8006,25 +8117,25 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="36" t="s">
+        <v>371</v>
+      </c>
+      <c r="O20" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="R20" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="S20" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="O20" s="37" t="s">
+      <c r="T20" s="18" t="s">
         <v>377</v>
-      </c>
-      <c r="P20" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q20" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="R20" s="17" t="s">
-        <v>380</v>
-      </c>
-      <c r="S20" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="T20" s="18" t="s">
-        <v>382</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -8047,25 +8158,25 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="36" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="O21" s="36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="P21" s="16" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="R21" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="S21" s="16" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="T21" s="16" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
@@ -8084,31 +8195,31 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="36" t="s">
+        <v>380</v>
+      </c>
+      <c r="O22" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q22" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="S22" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="T22" s="16" t="s">
         <v>385</v>
-      </c>
-      <c r="O22" s="36" t="s">
-        <v>315</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>388</v>
-      </c>
-      <c r="S22" s="16" t="s">
-        <v>389</v>
-      </c>
-      <c r="T22" s="16" t="s">
-        <v>390</v>
       </c>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
@@ -8127,7 +8238,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -8152,7 +8263,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -8200,7 +8311,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -8227,7 +8338,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="36" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>

</xml_diff>